<commit_message>
Queue item add logic
</commit_message>
<xml_diff>
--- a/Rules.xlsx
+++ b/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C3704D-8811-4DE8-A36F-2281B08C4314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A995653-B319-4F0A-B425-28C8B030B5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3195" yWindow="3105" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{F8A05525-B3EB-4424-9D4D-7345C82E46E0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -53,7 +53,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Tag2</t>
+  </si>
+  <si>
+    <t>no-reply@revature.net</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,14 +531,21 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F58BA2E6-0F06-4B29-BD52-8E29FBD5BC1B}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{A2D24F4D-B18E-4911-9D86-48C8FF23AABA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed rules and process
</commit_message>
<xml_diff>
--- a/Rules.xlsx
+++ b/Rules.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\JewlzAndTheBoyz-EmailCategorizationBot-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A995653-B319-4F0A-B425-28C8B030B5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301DDEFF-D3FD-4485-85F3-71B74F263885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3105" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{F8A05525-B3EB-4424-9D4D-7345C82E46E0}"/>
+    <workbookView xWindow="63570" yWindow="2460" windowWidth="17280" windowHeight="9000" activeTab="2" xr2:uid="{F8A05525-B3EB-4424-9D4D-7345C82E46E0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Julie" sheetId="1" r:id="rId1"/>
-    <sheet name="Michael" sheetId="2" r:id="rId2"/>
-    <sheet name="Brian" sheetId="3" r:id="rId3"/>
+    <sheet name="Julie" sheetId="4" r:id="rId1"/>
+    <sheet name="Michael" sheetId="5" r:id="rId2"/>
+    <sheet name="Brian" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,52 +27,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Attachment</t>
-  </si>
-  <si>
-    <t>Tag1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>foleyb25@gmail.com</t>
   </si>
   <si>
-    <t>Sender</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Tag2</t>
-  </si>
-  <si>
-    <t>no-reply@revature.net</t>
+    <t>Foley</t>
+  </si>
+  <si>
+    <t>important</t>
+  </si>
+  <si>
+    <t>Tag Name</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>trump</t>
+  </si>
+  <si>
+    <t>orders@oe.target.com</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>Attach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,12 +111,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,27 +430,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2198946B-4FDE-40EB-B23F-0690889DA236}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C594C03D-EEF8-416F-BD6B-CF19B76CC1D2}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="4" max="4" width="10.47265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
         <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -456,27 +470,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2A770A-DD95-4D14-9E4E-910F5DB43807}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC671B8-FB17-4529-998D-C1A952BEB850}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.3125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -485,67 +518,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7579FC0-7D76-4B2C-92F0-D877FEFFCE5A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5EDF72-B3ED-4046-B6C4-FCC85CF1F92B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F58BA2E6-0F06-4B29-BD52-8E29FBD5BC1B}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{A2D24F4D-B18E-4911-9D86-48C8FF23AABA}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{223C73C4-4814-4FC7-B812-17214907490D}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0EF9098F-07FB-4D14-BA86-88BBD6CF3B0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>